<commit_message>
started to write tests... and realized the logic uses too much gas. i have to make changes
</commit_message>
<xml_diff>
--- a/Book4.xlsx
+++ b/Book4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mickaelgermemont/Work-Mick/ether-dev/src/github.com/swellander/black_dapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC71893-7D93-D34F-98CF-D657D3087EF5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68368B20-4A3F-464D-84A7-514FE72272CC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3580" yWindow="2560" windowWidth="27240" windowHeight="16440" xr2:uid="{251046F0-FC18-7F4B-84DC-BCDEEE3032A8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>ACE</t>
   </si>
@@ -52,6 +52,18 @@
   </si>
   <si>
     <t>min number of cards</t>
+  </si>
+  <si>
+    <t>clubs mod 13</t>
+  </si>
+  <si>
+    <t>diamonds mod 13</t>
+  </si>
+  <si>
+    <t>hearts mod13</t>
+  </si>
+  <si>
+    <t>spades mod13</t>
   </si>
 </sst>
 </file>
@@ -403,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{627C588C-045D-504A-82C2-0E27673A4078}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -414,7 +426,7 @@
     <col min="7" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>4</v>
       </c>
@@ -433,8 +445,20 @@
       <c r="H1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -442,6 +466,7 @@
         <v>0</v>
       </c>
       <c r="C2">
+        <f>B14+1</f>
         <v>13</v>
       </c>
       <c r="D2">
@@ -455,8 +480,24 @@
       <c r="H2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J2">
+        <f>MOD(B2,13)</f>
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <f>MOD(C2,13)</f>
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <f>MOD(D2,13)</f>
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <f>MOD(E2,13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -482,8 +523,24 @@
       <c r="H3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J3">
+        <f>MOD(B3,13)</f>
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <f>MOD(C3,13)</f>
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <f>MOD(D3,13)</f>
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M14" si="0">MOD(E3,13)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -509,8 +566,24 @@
       <c r="H4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J4">
+        <f>MOD(B4,13)</f>
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <f>MOD(C4,13)</f>
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <f>MOD(D4,13)</f>
+        <v>2</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -536,8 +609,24 @@
       <c r="H5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J5">
+        <f>MOD(B5,13)</f>
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <f>MOD(C5,13)</f>
+        <v>3</v>
+      </c>
+      <c r="L5">
+        <f t="shared" ref="L5:L14" si="1">MOD(D5,13)</f>
+        <v>3</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -563,8 +652,24 @@
       <c r="H6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J6">
+        <f>MOD(B6,13)</f>
+        <v>4</v>
+      </c>
+      <c r="K6">
+        <f>MOD(C6,13)</f>
+        <v>4</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -590,8 +695,24 @@
       <c r="H7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J7">
+        <f>MOD(B7,13)</f>
+        <v>5</v>
+      </c>
+      <c r="K7">
+        <f>MOD(C7,13)</f>
+        <v>5</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -617,8 +738,24 @@
       <c r="H8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J8">
+        <f>MOD(B8,13)</f>
+        <v>6</v>
+      </c>
+      <c r="K8">
+        <f>MOD(C8,13)</f>
+        <v>6</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -644,8 +781,24 @@
       <c r="H9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J9">
+        <f>MOD(B9,13)</f>
+        <v>7</v>
+      </c>
+      <c r="K9">
+        <f>MOD(C9,13)</f>
+        <v>7</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -671,8 +824,24 @@
       <c r="H10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J10">
+        <f>MOD(B10,13)</f>
+        <v>8</v>
+      </c>
+      <c r="K10">
+        <f>MOD(C10,13)</f>
+        <v>8</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -695,8 +864,24 @@
       <c r="H11">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J11">
+        <f>MOD(B11,13)</f>
+        <v>9</v>
+      </c>
+      <c r="K11">
+        <f>MOD(C11,13)</f>
+        <v>9</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -719,8 +904,24 @@
       <c r="H12">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J12">
+        <f>MOD(B12,13)</f>
+        <v>10</v>
+      </c>
+      <c r="K12">
+        <f>MOD(C12,13)</f>
+        <v>10</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -740,8 +941,24 @@
         <f>E12+1</f>
         <v>50</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J13">
+        <f>MOD(B13,13)</f>
+        <v>11</v>
+      </c>
+      <c r="K13">
+        <f>MOD(C13,13)</f>
+        <v>11</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -761,8 +978,24 @@
         <f>E13+1</f>
         <v>51</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J14">
+        <f>MOD(B14,13)</f>
+        <v>12</v>
+      </c>
+      <c r="K14">
+        <f>MOD(C14,13)</f>
+        <v>12</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G15">
         <f>SUM(G3:G14)</f>
         <v>20</v>

</xml_diff>